<commit_message>
Update for wind and grid
wind and grid are now green leds instead of rgbs. code updated and
commented accordingly.
</commit_message>
<xml_diff>
--- a/ArduinoSerialCommands.xlsx
+++ b/ArduinoSerialCommands.xlsx
@@ -13,8 +13,66 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="D12" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Relic action from when item used rgb led. Can be used in future.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D15" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Relic action from when item used rgb led. Can be used in future.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="28">
   <si>
     <t>Command</t>
   </si>
@@ -88,29 +146,42 @@
     <t>Wind</t>
   </si>
   <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t>Available</t>
-  </si>
-  <si>
     <t>Used</t>
   </si>
   <si>
     <t>Grid</t>
+  </si>
+  <si>
+    <t>Pin</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -438,11 +509,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -450,7 +521,7 @@
     <col min="1" max="3" width="23.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -460,8 +531,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -471,8 +545,11 @@
       <c r="C2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -482,8 +559,11 @@
       <c r="C3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -493,8 +573,11 @@
       <c r="C4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -504,8 +587,11 @@
       <c r="C5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -515,8 +601,11 @@
       <c r="C6" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -526,8 +615,11 @@
       <c r="C7" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -537,8 +629,11 @@
       <c r="C8" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -548,8 +643,11 @@
       <c r="C9" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -557,10 +655,13 @@
         <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="D10">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -568,10 +669,13 @@
         <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="D11">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -579,43 +683,56 @@
         <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="D12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="D13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C14" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="D14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
       <c r="B15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" t="s">
         <v>27</v>
-      </c>
-      <c r="C15" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>